<commit_message>
Add support for constant sheet in Excel generation
- Updated proto parser to handle sheet fields without 'repeated' keyword.
- Implemented special formatting for constant sheets in Excel output.
</commit_message>
<xml_diff>
--- a/internal/pbz/test/测试配置读取.xlsx
+++ b/internal/pbz/test/测试配置读取.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C039407-D13A-B149-855B-9835FD4AC3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="true"/>
   <bookViews>
-    <workbookView xWindow="68640" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68640" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="测试页签1" sheetId="2" r:id="rId1"/>
     <sheet name="test_sheet_2" sheetId="3" r:id="rId2"/>
+    <sheet name="测试常量页签" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>测试字段1</t>
   </si>
@@ -25,13 +25,27 @@
   </si>
   <si>
     <t>test_field_3</t>
+  </si>
+  <si>
+    <t>测试常量字段1</t>
+  </si>
+  <si>
+    <t>测试常量字段2</t>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,14 +79,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -85,120 +100,120 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
+<theme xmlns="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <themeElements>
+    <clrScheme name="Office">
+      <dk1>
+        <sysClr val="windowText" lastClr="000000"/>
+      </dk1>
+      <lt1>
+        <sysClr val="window" lastClr="FFFFFF"/>
+      </lt1>
+      <dk2>
+        <srgbClr val="44546A"/>
+      </dk2>
+      <lt2>
+        <srgbClr val="E7E6E6"/>
+      </lt2>
+      <accent1>
+        <srgbClr val="5B9BD5"/>
+      </accent1>
+      <accent2>
+        <srgbClr val="ED7D31"/>
+      </accent2>
+      <accent3>
+        <srgbClr val="A5A5A5"/>
+      </accent3>
+      <accent4>
+        <srgbClr val="FFC000"/>
+      </accent4>
+      <accent5>
+        <srgbClr val="4472C4"/>
+      </accent5>
+      <accent6>
+        <srgbClr val="70AD47"/>
+      </accent6>
+      <hlink>
+        <srgbClr val="0563C1"/>
+      </hlink>
+      <folHlink>
+        <srgbClr val="954F72"/>
+      </folHlink>
+    </clrScheme>
+    <fontScheme name="Office">
+      <majorFont>
+        <latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="游ゴシック Light"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线 Light"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Times New Roman"/>
+        <font script="Hebr" typeface="Times New Roman"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="MoolBoran"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Times New Roman"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+      </majorFont>
+      <minorFont>
+        <latin typeface="Calibri" panose="020F0502020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="游ゴシック"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="等线"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Arial"/>
+        <font script="Hebr" typeface="Arial"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="DaunPenh"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Arial"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+      </minorFont>
+    </fontScheme>
+    <fmtScheme name="Office">
+      <fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -254,8 +269,8 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
+      </fillStyleLst>
+      <lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -277,8 +292,8 @@
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
+      </lnStyleLst>
+      <effectStyleLst>
         <a:effectStyle>
           <a:effectLst/>
         </a:effectStyle>
@@ -294,8 +309,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
+      </effectStyleLst>
+      <bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -332,20 +347,20 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
+      </bgFillStyleLst>
+    </fmtScheme>
+  </themeElements>
+  <objectDefaults/>
+  <extraClrSchemeLst/>
+</theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -436,4 +451,63 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>